<commit_message>
Start adding the filtes for the Ceramides where the MS/MS are checked if are [M+H]+ or [M+H-H2O]+
Comments:
- The filter works but it over filters the results need to check it again
- change the names of parameters of the function ions_control_cer from scoeHunter.py since is copy paste of the ions_control_check
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/2-Score_weight_Cer.xlsx
+++ b/ConfigurationFiles/2-Score_weight_Cer.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12651"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="5" r:id="rId1"/>
+    <sheet name="Cer" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -442,16 +442,16 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.07421875" customWidth="1"/>
-    <col min="5" max="5" width="40.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -468,12 +468,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -490,7 +490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -507,7 +507,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -524,7 +524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -541,12 +541,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -563,7 +563,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -580,7 +580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -597,7 +597,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -614,7 +614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -631,7 +631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -648,7 +648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -665,7 +665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -682,12 +682,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -704,7 +704,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -721,7 +721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -738,7 +738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -755,7 +755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -772,7 +772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -789,7 +789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -806,7 +806,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -823,7 +823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -840,7 +840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>

</xml_diff>